<commit_message>
correction balises vides type <DateMajIntervenant/>
</commit_message>
<xml_diff>
--- a/dev/modèle bon de commande vierge/modele_bdc_vierge_ugve.xlsx
+++ b/dev/modèle bon de commande vierge/modele_bdc_vierge_ugve.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28129"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="29426"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\workspace\LibreSQE\dev\modèle bon de commande vierge\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2F4B855F-CB10-4036-99E5-E2F0B030FF90}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B4DE2729-9ECA-4D9D-BA54-E4FF31897F8C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="quantitatif" sheetId="9" r:id="rId1"/>
@@ -19,7 +19,7 @@
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">trame!$A$1:$C$16</definedName>
-    <definedName name="_xlnm.Print_Area" localSheetId="1">programme!$A$1:$I$38</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="1">programme!$A$1:$J$43</definedName>
     <definedName name="_xlnm.Print_Area" localSheetId="0">quantitatif!$A$1:$F$62</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
@@ -979,7 +979,7 @@
   </sheetPr>
   <dimension ref="A1:F57"/>
   <sheetViews>
-    <sheetView tabSelected="1" view="pageBreakPreview" topLeftCell="A19" zoomScaleNormal="100" zoomScaleSheetLayoutView="100" workbookViewId="0">
+    <sheetView view="pageBreakPreview" topLeftCell="A19" zoomScaleNormal="100" zoomScaleSheetLayoutView="100" workbookViewId="0">
       <selection activeCell="F52" sqref="F52"/>
     </sheetView>
   </sheetViews>
@@ -1587,7 +1587,7 @@
       </c>
       <c r="C57" s="41">
         <f ca="1">TODAY()</f>
-        <v>45632</v>
+        <v>46029</v>
       </c>
     </row>
   </sheetData>
@@ -1614,10 +1614,10 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:I38"/>
+  <dimension ref="A1:J43"/>
   <sheetViews>
-    <sheetView view="pageBreakPreview" zoomScale="60" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F31" sqref="F31"/>
+    <sheetView tabSelected="1" view="pageBreakPreview" zoomScale="60" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="J3" sqref="J3:J43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1632,7 +1632,7 @@
     <col min="9" max="9" width="11.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B1" s="18" t="s">
         <v>35</v>
       </c>
@@ -1648,7 +1648,7 @@
       <c r="H1" s="43"/>
       <c r="I1" s="43"/>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B2" s="10" t="s">
         <v>36</v>
       </c>
@@ -1656,7 +1656,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="3" spans="1:9" s="17" customFormat="1" ht="149.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:10" s="17" customFormat="1" ht="149.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="16" t="s">
         <v>33</v>
       </c>
@@ -1668,8 +1668,9 @@
       <c r="G3" s="16"/>
       <c r="H3" s="16"/>
       <c r="I3" s="16"/>
-    </row>
-    <row r="4" spans="1:9" ht="18.75" x14ac:dyDescent="0.25">
+      <c r="J3" s="16"/>
+    </row>
+    <row r="4" spans="1:10" ht="18.75" x14ac:dyDescent="0.25">
       <c r="A4" s="11"/>
       <c r="B4" s="12"/>
       <c r="C4" s="12"/>
@@ -1679,8 +1680,9 @@
       <c r="G4" s="14"/>
       <c r="H4" s="14"/>
       <c r="I4" s="14"/>
-    </row>
-    <row r="5" spans="1:9" ht="18.75" x14ac:dyDescent="0.25">
+      <c r="J4" s="14"/>
+    </row>
+    <row r="5" spans="1:10" ht="18.75" x14ac:dyDescent="0.25">
       <c r="A5" s="11"/>
       <c r="B5" s="12"/>
       <c r="C5" s="12"/>
@@ -1690,8 +1692,9 @@
       <c r="G5" s="14"/>
       <c r="H5" s="14"/>
       <c r="I5" s="14"/>
-    </row>
-    <row r="6" spans="1:9" ht="18.75" x14ac:dyDescent="0.25">
+      <c r="J5" s="14"/>
+    </row>
+    <row r="6" spans="1:10" ht="18.75" x14ac:dyDescent="0.25">
       <c r="A6" s="11"/>
       <c r="B6" s="12"/>
       <c r="C6" s="12"/>
@@ -1701,8 +1704,9 @@
       <c r="G6" s="14"/>
       <c r="H6" s="14"/>
       <c r="I6" s="14"/>
-    </row>
-    <row r="7" spans="1:9" ht="18.75" x14ac:dyDescent="0.25">
+      <c r="J6" s="14"/>
+    </row>
+    <row r="7" spans="1:10" ht="18.75" x14ac:dyDescent="0.25">
       <c r="A7" s="11"/>
       <c r="B7" s="15"/>
       <c r="C7" s="15"/>
@@ -1712,8 +1716,9 @@
       <c r="G7" s="14"/>
       <c r="H7" s="14"/>
       <c r="I7" s="14"/>
-    </row>
-    <row r="8" spans="1:9" ht="18.75" x14ac:dyDescent="0.25">
+      <c r="J7" s="14"/>
+    </row>
+    <row r="8" spans="1:10" ht="18.75" x14ac:dyDescent="0.25">
       <c r="A8" s="11"/>
       <c r="B8" s="15"/>
       <c r="C8" s="15"/>
@@ -1723,8 +1728,9 @@
       <c r="G8" s="14"/>
       <c r="H8" s="14"/>
       <c r="I8" s="14"/>
-    </row>
-    <row r="9" spans="1:9" ht="18.75" x14ac:dyDescent="0.25">
+      <c r="J8" s="14"/>
+    </row>
+    <row r="9" spans="1:10" ht="18.75" x14ac:dyDescent="0.25">
       <c r="A9" s="11"/>
       <c r="B9" s="12"/>
       <c r="C9" s="12"/>
@@ -1734,8 +1740,9 @@
       <c r="G9" s="14"/>
       <c r="H9" s="14"/>
       <c r="I9" s="14"/>
-    </row>
-    <row r="10" spans="1:9" ht="18.75" x14ac:dyDescent="0.25">
+      <c r="J9" s="14"/>
+    </row>
+    <row r="10" spans="1:10" ht="18.75" x14ac:dyDescent="0.25">
       <c r="A10" s="11"/>
       <c r="B10" s="12"/>
       <c r="C10" s="12"/>
@@ -1745,8 +1752,9 @@
       <c r="G10" s="14"/>
       <c r="H10" s="14"/>
       <c r="I10" s="14"/>
-    </row>
-    <row r="11" spans="1:9" ht="18.75" x14ac:dyDescent="0.25">
+      <c r="J10" s="14"/>
+    </row>
+    <row r="11" spans="1:10" ht="18.75" x14ac:dyDescent="0.25">
       <c r="A11" s="11"/>
       <c r="B11" s="12"/>
       <c r="C11" s="12"/>
@@ -1756,8 +1764,9 @@
       <c r="G11" s="14"/>
       <c r="H11" s="14"/>
       <c r="I11" s="14"/>
-    </row>
-    <row r="12" spans="1:9" ht="18.75" x14ac:dyDescent="0.25">
+      <c r="J11" s="14"/>
+    </row>
+    <row r="12" spans="1:10" ht="18.75" x14ac:dyDescent="0.25">
       <c r="A12" s="11"/>
       <c r="B12" s="12"/>
       <c r="C12" s="12"/>
@@ -1767,8 +1776,9 @@
       <c r="G12" s="14"/>
       <c r="H12" s="14"/>
       <c r="I12" s="14"/>
-    </row>
-    <row r="13" spans="1:9" ht="18.75" x14ac:dyDescent="0.25">
+      <c r="J12" s="14"/>
+    </row>
+    <row r="13" spans="1:10" ht="18.75" x14ac:dyDescent="0.25">
       <c r="A13" s="11"/>
       <c r="B13" s="12"/>
       <c r="C13" s="12"/>
@@ -1778,8 +1788,9 @@
       <c r="G13" s="14"/>
       <c r="H13" s="14"/>
       <c r="I13" s="14"/>
-    </row>
-    <row r="14" spans="1:9" ht="18.75" x14ac:dyDescent="0.25">
+      <c r="J13" s="14"/>
+    </row>
+    <row r="14" spans="1:10" ht="18.75" x14ac:dyDescent="0.25">
       <c r="A14" s="11"/>
       <c r="B14" s="12"/>
       <c r="C14" s="12"/>
@@ -1789,8 +1800,9 @@
       <c r="G14" s="14"/>
       <c r="H14" s="14"/>
       <c r="I14" s="14"/>
-    </row>
-    <row r="15" spans="1:9" ht="18.75" x14ac:dyDescent="0.25">
+      <c r="J14" s="14"/>
+    </row>
+    <row r="15" spans="1:10" ht="18.75" x14ac:dyDescent="0.25">
       <c r="A15" s="11"/>
       <c r="B15" s="12"/>
       <c r="C15" s="12"/>
@@ -1800,8 +1812,9 @@
       <c r="G15" s="14"/>
       <c r="H15" s="14"/>
       <c r="I15" s="14"/>
-    </row>
-    <row r="16" spans="1:9" ht="18.75" x14ac:dyDescent="0.25">
+      <c r="J15" s="14"/>
+    </row>
+    <row r="16" spans="1:10" ht="18.75" x14ac:dyDescent="0.25">
       <c r="A16" s="11"/>
       <c r="B16" s="12"/>
       <c r="C16" s="12"/>
@@ -1811,8 +1824,9 @@
       <c r="G16" s="14"/>
       <c r="H16" s="14"/>
       <c r="I16" s="14"/>
-    </row>
-    <row r="17" spans="1:9" ht="18.75" x14ac:dyDescent="0.25">
+      <c r="J16" s="14"/>
+    </row>
+    <row r="17" spans="1:10" ht="18.75" x14ac:dyDescent="0.25">
       <c r="A17" s="11"/>
       <c r="B17" s="12"/>
       <c r="C17" s="12"/>
@@ -1822,8 +1836,9 @@
       <c r="G17" s="14"/>
       <c r="H17" s="14"/>
       <c r="I17" s="14"/>
-    </row>
-    <row r="18" spans="1:9" ht="18.75" x14ac:dyDescent="0.25">
+      <c r="J17" s="14"/>
+    </row>
+    <row r="18" spans="1:10" ht="18.75" x14ac:dyDescent="0.25">
       <c r="A18" s="11"/>
       <c r="B18" s="12"/>
       <c r="C18" s="12"/>
@@ -1833,8 +1848,9 @@
       <c r="G18" s="14"/>
       <c r="H18" s="14"/>
       <c r="I18" s="14"/>
-    </row>
-    <row r="19" spans="1:9" ht="18.75" x14ac:dyDescent="0.25">
+      <c r="J18" s="14"/>
+    </row>
+    <row r="19" spans="1:10" ht="18.75" x14ac:dyDescent="0.25">
       <c r="A19" s="11"/>
       <c r="B19" s="12"/>
       <c r="C19" s="12"/>
@@ -1844,8 +1860,9 @@
       <c r="G19" s="14"/>
       <c r="H19" s="14"/>
       <c r="I19" s="14"/>
-    </row>
-    <row r="20" spans="1:9" ht="18.75" x14ac:dyDescent="0.25">
+      <c r="J19" s="14"/>
+    </row>
+    <row r="20" spans="1:10" ht="18.75" x14ac:dyDescent="0.25">
       <c r="A20" s="11"/>
       <c r="B20" s="12"/>
       <c r="C20" s="12"/>
@@ -1855,8 +1872,9 @@
       <c r="G20" s="14"/>
       <c r="H20" s="14"/>
       <c r="I20" s="14"/>
-    </row>
-    <row r="21" spans="1:9" ht="18.75" x14ac:dyDescent="0.25">
+      <c r="J20" s="14"/>
+    </row>
+    <row r="21" spans="1:10" ht="18.75" x14ac:dyDescent="0.25">
       <c r="A21" s="11"/>
       <c r="B21" s="12"/>
       <c r="C21" s="12"/>
@@ -1866,8 +1884,9 @@
       <c r="G21" s="14"/>
       <c r="H21" s="14"/>
       <c r="I21" s="14"/>
-    </row>
-    <row r="22" spans="1:9" ht="18.75" x14ac:dyDescent="0.25">
+      <c r="J21" s="14"/>
+    </row>
+    <row r="22" spans="1:10" ht="18.75" x14ac:dyDescent="0.25">
       <c r="A22" s="11"/>
       <c r="B22" s="12"/>
       <c r="C22" s="12"/>
@@ -1877,8 +1896,9 @@
       <c r="G22" s="14"/>
       <c r="H22" s="14"/>
       <c r="I22" s="14"/>
-    </row>
-    <row r="23" spans="1:9" ht="18.75" x14ac:dyDescent="0.25">
+      <c r="J22" s="14"/>
+    </row>
+    <row r="23" spans="1:10" ht="18.75" x14ac:dyDescent="0.25">
       <c r="A23" s="11"/>
       <c r="B23" s="12"/>
       <c r="C23" s="12"/>
@@ -1888,8 +1908,9 @@
       <c r="G23" s="14"/>
       <c r="H23" s="14"/>
       <c r="I23" s="14"/>
-    </row>
-    <row r="24" spans="1:9" ht="18.75" x14ac:dyDescent="0.25">
+      <c r="J23" s="14"/>
+    </row>
+    <row r="24" spans="1:10" ht="18.75" x14ac:dyDescent="0.25">
       <c r="A24" s="11"/>
       <c r="B24" s="12"/>
       <c r="C24" s="12"/>
@@ -1899,8 +1920,9 @@
       <c r="G24" s="14"/>
       <c r="H24" s="14"/>
       <c r="I24" s="14"/>
-    </row>
-    <row r="25" spans="1:9" ht="18.75" x14ac:dyDescent="0.25">
+      <c r="J24" s="14"/>
+    </row>
+    <row r="25" spans="1:10" ht="18.75" x14ac:dyDescent="0.25">
       <c r="A25" s="11"/>
       <c r="B25" s="12"/>
       <c r="C25" s="12"/>
@@ -1910,8 +1932,9 @@
       <c r="G25" s="14"/>
       <c r="H25" s="14"/>
       <c r="I25" s="14"/>
-    </row>
-    <row r="26" spans="1:9" ht="18.75" x14ac:dyDescent="0.25">
+      <c r="J25" s="14"/>
+    </row>
+    <row r="26" spans="1:10" ht="18.75" x14ac:dyDescent="0.25">
       <c r="A26" s="11"/>
       <c r="B26" s="12"/>
       <c r="C26" s="12"/>
@@ -1921,8 +1944,9 @@
       <c r="G26" s="14"/>
       <c r="H26" s="14"/>
       <c r="I26" s="14"/>
-    </row>
-    <row r="27" spans="1:9" ht="18.75" x14ac:dyDescent="0.25">
+      <c r="J26" s="14"/>
+    </row>
+    <row r="27" spans="1:10" ht="18.75" x14ac:dyDescent="0.25">
       <c r="A27" s="11"/>
       <c r="B27" s="12"/>
       <c r="C27" s="12"/>
@@ -1932,8 +1956,9 @@
       <c r="G27" s="14"/>
       <c r="H27" s="14"/>
       <c r="I27" s="14"/>
-    </row>
-    <row r="28" spans="1:9" ht="18.75" x14ac:dyDescent="0.25">
+      <c r="J27" s="14"/>
+    </row>
+    <row r="28" spans="1:10" ht="18.75" x14ac:dyDescent="0.25">
       <c r="A28" s="11"/>
       <c r="B28" s="12"/>
       <c r="C28" s="12"/>
@@ -1943,8 +1968,9 @@
       <c r="G28" s="14"/>
       <c r="H28" s="14"/>
       <c r="I28" s="14"/>
-    </row>
-    <row r="29" spans="1:9" ht="18.75" x14ac:dyDescent="0.25">
+      <c r="J28" s="14"/>
+    </row>
+    <row r="29" spans="1:10" ht="18.75" x14ac:dyDescent="0.25">
       <c r="A29" s="11"/>
       <c r="B29" s="12"/>
       <c r="C29" s="12"/>
@@ -1954,8 +1980,9 @@
       <c r="G29" s="14"/>
       <c r="H29" s="14"/>
       <c r="I29" s="14"/>
-    </row>
-    <row r="30" spans="1:9" ht="18.75" x14ac:dyDescent="0.25">
+      <c r="J29" s="14"/>
+    </row>
+    <row r="30" spans="1:10" ht="18.75" x14ac:dyDescent="0.25">
       <c r="A30" s="11"/>
       <c r="B30" s="12"/>
       <c r="C30" s="12"/>
@@ -1965,8 +1992,9 @@
       <c r="G30" s="14"/>
       <c r="H30" s="14"/>
       <c r="I30" s="14"/>
-    </row>
-    <row r="31" spans="1:9" ht="18.75" x14ac:dyDescent="0.25">
+      <c r="J30" s="14"/>
+    </row>
+    <row r="31" spans="1:10" ht="18.75" x14ac:dyDescent="0.25">
       <c r="A31" s="11"/>
       <c r="B31" s="12"/>
       <c r="C31" s="12"/>
@@ -1976,8 +2004,9 @@
       <c r="G31" s="14"/>
       <c r="H31" s="14"/>
       <c r="I31" s="14"/>
-    </row>
-    <row r="32" spans="1:9" ht="18.75" x14ac:dyDescent="0.25">
+      <c r="J31" s="14"/>
+    </row>
+    <row r="32" spans="1:10" ht="18.75" x14ac:dyDescent="0.25">
       <c r="A32" s="11"/>
       <c r="B32" s="12"/>
       <c r="C32" s="12"/>
@@ -1987,8 +2016,9 @@
       <c r="G32" s="14"/>
       <c r="H32" s="14"/>
       <c r="I32" s="14"/>
-    </row>
-    <row r="33" spans="1:9" ht="18.75" x14ac:dyDescent="0.25">
+      <c r="J32" s="14"/>
+    </row>
+    <row r="33" spans="1:10" ht="18.75" x14ac:dyDescent="0.25">
       <c r="A33" s="11"/>
       <c r="B33" s="12"/>
       <c r="C33" s="12"/>
@@ -1998,8 +2028,9 @@
       <c r="G33" s="14"/>
       <c r="H33" s="14"/>
       <c r="I33" s="14"/>
-    </row>
-    <row r="34" spans="1:9" ht="18.75" x14ac:dyDescent="0.25">
+      <c r="J33" s="14"/>
+    </row>
+    <row r="34" spans="1:10" ht="18.75" x14ac:dyDescent="0.25">
       <c r="A34" s="11"/>
       <c r="B34" s="12"/>
       <c r="C34" s="12"/>
@@ -2009,8 +2040,9 @@
       <c r="G34" s="14"/>
       <c r="H34" s="14"/>
       <c r="I34" s="14"/>
-    </row>
-    <row r="35" spans="1:9" ht="18.75" x14ac:dyDescent="0.25">
+      <c r="J34" s="14"/>
+    </row>
+    <row r="35" spans="1:10" ht="18.75" x14ac:dyDescent="0.25">
       <c r="A35" s="11"/>
       <c r="B35" s="12"/>
       <c r="C35" s="12"/>
@@ -2020,8 +2052,9 @@
       <c r="G35" s="14"/>
       <c r="H35" s="14"/>
       <c r="I35" s="14"/>
-    </row>
-    <row r="36" spans="1:9" ht="18.75" x14ac:dyDescent="0.25">
+      <c r="J35" s="14"/>
+    </row>
+    <row r="36" spans="1:10" ht="18.75" x14ac:dyDescent="0.25">
       <c r="A36" s="11"/>
       <c r="B36" s="12"/>
       <c r="C36" s="12"/>
@@ -2031,8 +2064,9 @@
       <c r="G36" s="14"/>
       <c r="H36" s="14"/>
       <c r="I36" s="14"/>
-    </row>
-    <row r="37" spans="1:9" ht="18.75" x14ac:dyDescent="0.25">
+      <c r="J36" s="14"/>
+    </row>
+    <row r="37" spans="1:10" ht="18.75" x14ac:dyDescent="0.25">
       <c r="A37" s="11"/>
       <c r="B37" s="12"/>
       <c r="C37" s="12"/>
@@ -2042,8 +2076,9 @@
       <c r="G37" s="14"/>
       <c r="H37" s="14"/>
       <c r="I37" s="14"/>
-    </row>
-    <row r="38" spans="1:9" ht="18.75" x14ac:dyDescent="0.25">
+      <c r="J37" s="14"/>
+    </row>
+    <row r="38" spans="1:10" ht="18.75" x14ac:dyDescent="0.25">
       <c r="A38" s="11"/>
       <c r="B38" s="12"/>
       <c r="C38" s="12"/>
@@ -2053,13 +2088,74 @@
       <c r="G38" s="14"/>
       <c r="H38" s="14"/>
       <c r="I38" s="14"/>
+      <c r="J38" s="14"/>
+    </row>
+    <row r="39" spans="1:10" ht="18.75" x14ac:dyDescent="0.25">
+      <c r="A39" s="11"/>
+      <c r="B39" s="12"/>
+      <c r="C39" s="12"/>
+      <c r="D39" s="12"/>
+      <c r="E39" s="13"/>
+      <c r="F39" s="14"/>
+      <c r="G39" s="14"/>
+      <c r="H39" s="14"/>
+      <c r="I39" s="14"/>
+      <c r="J39" s="14"/>
+    </row>
+    <row r="40" spans="1:10" ht="18.75" x14ac:dyDescent="0.25">
+      <c r="A40" s="11"/>
+      <c r="B40" s="12"/>
+      <c r="C40" s="12"/>
+      <c r="D40" s="12"/>
+      <c r="E40" s="13"/>
+      <c r="F40" s="14"/>
+      <c r="G40" s="14"/>
+      <c r="H40" s="14"/>
+      <c r="I40" s="14"/>
+      <c r="J40" s="14"/>
+    </row>
+    <row r="41" spans="1:10" ht="18.75" x14ac:dyDescent="0.25">
+      <c r="A41" s="11"/>
+      <c r="B41" s="12"/>
+      <c r="C41" s="12"/>
+      <c r="D41" s="12"/>
+      <c r="E41" s="13"/>
+      <c r="F41" s="14"/>
+      <c r="G41" s="14"/>
+      <c r="H41" s="14"/>
+      <c r="I41" s="14"/>
+      <c r="J41" s="14"/>
+    </row>
+    <row r="42" spans="1:10" ht="18.75" x14ac:dyDescent="0.25">
+      <c r="A42" s="11"/>
+      <c r="B42" s="12"/>
+      <c r="C42" s="12"/>
+      <c r="D42" s="12"/>
+      <c r="E42" s="13"/>
+      <c r="F42" s="14"/>
+      <c r="G42" s="14"/>
+      <c r="H42" s="14"/>
+      <c r="I42" s="14"/>
+      <c r="J42" s="14"/>
+    </row>
+    <row r="43" spans="1:10" ht="18.75" x14ac:dyDescent="0.25">
+      <c r="A43" s="11"/>
+      <c r="B43" s="12"/>
+      <c r="C43" s="12"/>
+      <c r="D43" s="12"/>
+      <c r="E43" s="13"/>
+      <c r="F43" s="14"/>
+      <c r="G43" s="14"/>
+      <c r="H43" s="14"/>
+      <c r="I43" s="14"/>
+      <c r="J43" s="14"/>
     </row>
   </sheetData>
   <mergeCells count="1">
     <mergeCell ref="G1:I1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" scale="59" orientation="landscape" r:id="rId1"/>
+  <pageSetup paperSize="9" scale="53" orientation="landscape" r:id="rId1"/>
   <drawing r:id="rId2"/>
 </worksheet>
 </file>
@@ -2317,6 +2413,15 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100B364072B9BF0174EACE646529BD3F8FC" ma:contentTypeVersion="14" ma:contentTypeDescription="Crée un document." ma:contentTypeScope="" ma:versionID="0a61469fa4392fe95df6df9ebb4bd246">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns3="2efdd341-56d0-41e7-aab3-73531d8de268" xmlns:ns4="283c0d33-edfc-4847-af07-30bb862e3054" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="ce621300719ead46a930f93492683fbc" ns3:_="" ns4:_="">
     <xsd:import namespace="2efdd341-56d0-41e7-aab3-73531d8de268"/>
@@ -2545,22 +2650,21 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement/>
 </p:properties>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{240AF456-82BA-4AF0-AA0F-2057DA65B299}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{541E0AED-18F9-4FA5-A843-11A8B9552700}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -2579,7 +2683,7 @@
 </ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{DF16ACF2-37E9-4949-9A93-88A3A015DDE8}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
@@ -2594,12 +2698,4 @@
     <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{240AF456-82BA-4AF0-AA0F-2057DA65B299}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>